<commit_message>
Updated Time Log - Boray
</commit_message>
<xml_diff>
--- a/project-planning/timelogs/Boray_Time_Log.xlsx
+++ b/project-planning/timelogs/Boray_Time_Log.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Time Log </t>
   </si>
@@ -52,13 +52,19 @@
   </si>
   <si>
     <t>-Discussed risk management, role division and possible improvements on vision document with the team. 
--Developed the vision document to its latest version after getting feedback from the team and the professor</t>
+-Developed the vision document to its latest version, also made a new file 'Non-Functional Requirements List'</t>
+  </si>
+  <si>
+    <t>-Meeting with the team, discussed the toolchain, reviewed the other member's works.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d.m"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="12.0"/>
@@ -129,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -170,6 +176,9 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -502,7 +511,7 @@
         <v>45938</v>
       </c>
       <c r="E7" s="13">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>11</v>
@@ -545,7 +554,7 @@
         <v>45945</v>
       </c>
       <c r="E8" s="13">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>12</v>
@@ -587,8 +596,12 @@
         <f t="shared" si="2"/>
         <v>45952</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="14">
+        <v>45778.0</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -626,8 +639,8 @@
         <f t="shared" si="2"/>
         <v>45959</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -665,8 +678,8 @@
         <f t="shared" si="2"/>
         <v>45966</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -704,8 +717,8 @@
         <f t="shared" si="2"/>
         <v>45973</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -743,8 +756,8 @@
         <f t="shared" si="2"/>
         <v>45980</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -782,8 +795,8 @@
         <f t="shared" si="2"/>
         <v>45987</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -821,8 +834,8 @@
         <f t="shared" si="2"/>
         <v>45994</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -860,8 +873,8 @@
         <f t="shared" si="2"/>
         <v>46001</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -899,8 +912,8 @@
         <f t="shared" si="2"/>
         <v>46008</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -938,8 +951,8 @@
         <f t="shared" si="2"/>
         <v>46015</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -977,8 +990,8 @@
         <f t="shared" si="2"/>
         <v>46022</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -1016,8 +1029,8 @@
         <f t="shared" si="2"/>
         <v>46029</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -1055,8 +1068,8 @@
         <f t="shared" si="2"/>
         <v>46036</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -1094,8 +1107,8 @@
         <f t="shared" si="2"/>
         <v>46043</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>

</xml_diff>